<commit_message>
fix admin report mlodn
</commit_message>
<xml_diff>
--- a/templates/mlo/mlodn.xlsx
+++ b/templates/mlo/mlodn.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27645" windowHeight="12840" activeTab="1"/>
+    <workbookView windowWidth="27735" windowHeight="15075"/>
   </bookViews>
   <sheets>
     <sheet name="Федеральная льгота" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>Мониторинг обеспеченности детского населения ФЕДЕРАЛЬНАЯ ЛЬГОТА</t>
   </si>
@@ -23,6 +24,9 @@
     <t>${date}</t>
   </si>
   <si>
+    <t>Дата</t>
+  </si>
+  <si>
     <t>Муниципальное образование</t>
   </si>
   <si>
@@ -32,10 +36,10 @@
     <t>Обеспечено рецептов с 01.01.2015г (накопительно)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Находится рецептов на отсроченном обеспечении до 10 дней</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Находится  рецептов на отсроченном обеспечении  свыше 10 дней</t>
+    <t>Находится рецептов на отсроченном обеспечении до 10 дней</t>
+  </si>
+  <si>
+    <t>Находится  рецептов на отсроченном обеспечении  свыше 10 дней</t>
   </si>
   <si>
     <t>Кол-во</t>
@@ -50,16 +54,7 @@
     <t>(руб)</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>${table:grs.inputdate}</t>
   </si>
   <si>
     <t>${table:grs.username}</t>
@@ -104,10 +99,7 @@
     <t>Категория граждан</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>${table:rgrs.inputdate}</t>
   </si>
   <si>
     <t>${table:rgrs.username}</t>
@@ -154,12 +146,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-419]dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="dd.mm.yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-419]General"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -198,7 +190,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,29 +200,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="44"/>
+        <bgColor indexed="31"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor indexed="9"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
-        <bgColor indexed="64"/>
+        <bgColor indexed="49"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -248,21 +234,8 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -273,40 +246,25 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -322,20 +280,20 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -345,86 +303,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="58" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -770,258 +766,227 @@
   <sheetPr>
     <tabColor indexed="17"/>
   </sheetPr>
-  <dimension ref="A1:XFC13"/>
+  <dimension ref="A1:AMK8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="25.1416666666667" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.8583333333333" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5666666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.8583333333333" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.8583333333333" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17" style="2" customWidth="1"/>
-    <col min="7" max="1024" width="9.28333333333333" style="2" customWidth="1"/>
-    <col min="16384" max="16384" width="9.14166666666667" style="2"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="25.1416666666667" style="2"/>
+    <col min="3" max="3" width="18.85" style="2"/>
+    <col min="4" max="4" width="12.5583333333333" style="2"/>
+    <col min="5" max="5" width="26.85" style="2"/>
+    <col min="6" max="6" width="16.8583333333333" style="2"/>
+    <col min="7" max="7" width="17" style="2"/>
+    <col min="8" max="1026" width="9.28333333333333" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="2:6">
-      <c r="B1" s="2"/>
+    <row r="1" s="1" customFormat="1" spans="3:7">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="13.5" spans="1:6">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" ht="13.5" spans="1:1025">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="78.75" customHeight="1" spans="1:6">
+      <c r="AME2"/>
+      <c r="AMF2"/>
+      <c r="AMG2"/>
+      <c r="AMH2"/>
+      <c r="AMI2"/>
+      <c r="AMJ2"/>
+      <c r="AMK2"/>
+    </row>
+    <row r="3" ht="78.75" customHeight="1" spans="1:1025">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:6">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="AME3"/>
+      <c r="AMF3"/>
+      <c r="AMG3"/>
+      <c r="AMH3"/>
+      <c r="AMI3"/>
+      <c r="AMJ3"/>
+      <c r="AMK3"/>
+    </row>
+    <row r="4" ht="25.5" customHeight="1" spans="1:1025">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="13.5" spans="1:6">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>9</v>
       </c>
+      <c r="F4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AME4"/>
+      <c r="AMF4"/>
+      <c r="AMG4"/>
+      <c r="AMH4"/>
+      <c r="AMI4"/>
+      <c r="AMJ4"/>
+      <c r="AMK4"/>
+    </row>
+    <row r="5" ht="13.5" spans="1:1025">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="13.5" spans="1:6">
-      <c r="A6" s="20">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AME5"/>
+      <c r="AMF5"/>
+      <c r="AMG5"/>
+      <c r="AMH5"/>
+      <c r="AMI5"/>
+      <c r="AMJ5"/>
+      <c r="AMK5"/>
+    </row>
+    <row r="6" ht="13.5" spans="1:1025">
+      <c r="A6" s="23">
         <v>1</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="24">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="25">
+        <v>3</v>
+      </c>
+      <c r="D6" s="26">
+        <v>4</v>
+      </c>
+      <c r="E6" s="26">
+        <v>5</v>
+      </c>
+      <c r="F6" s="26">
+        <v>6</v>
+      </c>
+      <c r="G6" s="26">
+        <v>7</v>
+      </c>
+      <c r="AME6"/>
+      <c r="AMF6"/>
+      <c r="AMG6"/>
+      <c r="AMH6"/>
+      <c r="AMI6"/>
+      <c r="AMJ6"/>
+      <c r="AMK6"/>
+    </row>
+    <row r="7" ht="27" spans="1:1025">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="B7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="27" spans="1:6">
-      <c r="A7" s="22" t="s">
+      <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="E7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="F7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="G7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="AME7"/>
+      <c r="AMF7"/>
+      <c r="AMG7"/>
+      <c r="AMH7"/>
+      <c r="AMI7"/>
+      <c r="AMJ7"/>
+      <c r="AMK7"/>
+    </row>
+    <row r="8" ht="21" customHeight="1" spans="1:1025">
+      <c r="A8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:16383">
-      <c r="A8" s="23" t="s">
+      <c r="D8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="E8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="F8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="G8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="AMD8" s="1"/>
       <c r="AME8" s="1"/>
       <c r="AMF8" s="1"/>
       <c r="AMG8" s="1"/>
       <c r="AMH8" s="1"/>
       <c r="AMI8" s="1"/>
       <c r="AMJ8" s="1"/>
-      <c r="XEW8" s="2"/>
-      <c r="XEX8" s="2"/>
-      <c r="XEY8" s="2"/>
-      <c r="XEZ8" s="2"/>
-      <c r="XFA8" s="2"/>
-      <c r="XFB8" s="2"/>
-      <c r="XFC8" s="2"/>
-    </row>
-    <row r="9" spans="1018:16383">
-      <c r="AMD9" s="1"/>
-      <c r="AME9" s="1"/>
-      <c r="AMF9" s="1"/>
-      <c r="AMG9" s="1"/>
-      <c r="AMH9" s="1"/>
-      <c r="AMI9" s="1"/>
-      <c r="AMJ9" s="1"/>
-      <c r="XEW9" s="2"/>
-      <c r="XEX9" s="2"/>
-      <c r="XEY9" s="2"/>
-      <c r="XEZ9" s="2"/>
-      <c r="XFA9" s="2"/>
-      <c r="XFB9" s="2"/>
-      <c r="XFC9" s="2"/>
-    </row>
-    <row r="10" spans="1018:16383">
-      <c r="AMD10" s="1"/>
-      <c r="AME10" s="1"/>
-      <c r="AMF10" s="1"/>
-      <c r="AMG10" s="1"/>
-      <c r="AMH10" s="1"/>
-      <c r="AMI10" s="1"/>
-      <c r="AMJ10" s="1"/>
-      <c r="XEW10" s="2"/>
-      <c r="XEX10" s="2"/>
-      <c r="XEY10" s="2"/>
-      <c r="XEZ10" s="2"/>
-      <c r="XFA10" s="2"/>
-      <c r="XFB10" s="2"/>
-      <c r="XFC10" s="2"/>
-    </row>
-    <row r="11" spans="1018:16383">
-      <c r="AMD11" s="1"/>
-      <c r="AME11" s="1"/>
-      <c r="AMF11" s="1"/>
-      <c r="AMG11" s="1"/>
-      <c r="AMH11" s="1"/>
-      <c r="AMI11" s="1"/>
-      <c r="AMJ11" s="1"/>
-      <c r="XEW11" s="2"/>
-      <c r="XEX11" s="2"/>
-      <c r="XEY11" s="2"/>
-      <c r="XEZ11" s="2"/>
-      <c r="XFA11" s="2"/>
-      <c r="XFB11" s="2"/>
-      <c r="XFC11" s="2"/>
-    </row>
-    <row r="12" spans="1018:16383">
-      <c r="AMD12" s="1"/>
-      <c r="AME12" s="1"/>
-      <c r="AMF12" s="1"/>
-      <c r="AMG12" s="1"/>
-      <c r="AMH12" s="1"/>
-      <c r="AMI12" s="1"/>
-      <c r="AMJ12" s="1"/>
-      <c r="XEW12" s="2"/>
-      <c r="XEX12" s="2"/>
-      <c r="XEY12" s="2"/>
-      <c r="XEZ12" s="2"/>
-      <c r="XFA12" s="2"/>
-      <c r="XFB12" s="2"/>
-      <c r="XFC12" s="2"/>
-    </row>
-    <row r="13" spans="1018:16383">
-      <c r="AMD13" s="1"/>
-      <c r="AME13" s="1"/>
-      <c r="AMF13" s="1"/>
-      <c r="AMG13" s="1"/>
-      <c r="AMH13" s="1"/>
-      <c r="AMI13" s="1"/>
-      <c r="AMJ13" s="1"/>
-      <c r="XEW13" s="2"/>
-      <c r="XEX13" s="2"/>
-      <c r="XEY13" s="2"/>
-      <c r="XEZ13" s="2"/>
-      <c r="XFA13" s="2"/>
-      <c r="XFB13" s="2"/>
-      <c r="XFC13" s="2"/>
+      <c r="AMK8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:D3"/>
+  <mergeCells count="4">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageMargins left="0.698611111111111" right="0.698611111111111" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1032,190 +997,207 @@
     <tabColor indexed="13"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="28.1416666666667" style="2" customWidth="1"/>
-    <col min="2" max="2" width="43.1416666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5666666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.5666666666667" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5666666666667" style="2" customWidth="1"/>
-    <col min="8" max="1023" width="9.28333333333333" style="2" customWidth="1"/>
-    <col min="16384" max="16384" width="9.14166666666667" style="2"/>
+    <col min="1" max="1" width="28.1416666666667"/>
+    <col min="2" max="2" width="28.1416666666667" style="2"/>
+    <col min="3" max="3" width="43.1416666666667" style="2"/>
+    <col min="4" max="4" width="12.5583333333333" style="2"/>
+    <col min="5" max="5" width="17.5666666666667" style="2"/>
+    <col min="6" max="6" width="16" style="2"/>
+    <col min="7" max="7" width="17" style="2"/>
+    <col min="8" max="8" width="16.5666666666667" style="2"/>
+    <col min="9" max="1025" width="9.28333333333333" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
-      <c r="A1" s="2"/>
+    <row r="1" s="1" customFormat="1" spans="2:8">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
-      <c r="A2" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="2:8">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:7">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B3"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="17" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="78.75" customHeight="1" spans="1:7">
+    <row r="4" ht="78.75" customHeight="1" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="27" spans="1:7">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="5" ht="27" spans="1:8">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="13.5" spans="1:7">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>9</v>
       </c>
+      <c r="G5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" spans="1:8">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="13.5" spans="1:7">
-      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" spans="1:8">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11">
+        <v>6</v>
+      </c>
+      <c r="G7" s="11">
+        <v>7</v>
+      </c>
+      <c r="H7" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="27" spans="1:8">
+      <c r="A8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="9" t="s">
+      <c r="D8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9">
-        <v>3</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="9">
-        <v>4</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="27" spans="1:7">
-      <c r="A8" s="10" t="s">
+      <c r="E8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="F8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="G8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="H8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="12" t="s">
+    </row>
+    <row r="9" ht="28" customHeight="1" spans="1:8">
+      <c r="A9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="D9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="E9" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" ht="13.5" spans="1:7">
-      <c r="A9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="F9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="G9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="H9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
+    </row>
+    <row r="10" ht="24" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D4:E4"/>
+  <mergeCells count="5">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
   </mergeCells>
-  <pageMargins left="0.314583333333333" right="0.314583333333333" top="0.196527777777778" bottom="0.156944444444444" header="0.314583333333333" footer="0.314583333333333"/>
-  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="landscape"/>
+  <pageMargins left="0.313888888888889" right="0.313888888888889" top="0.196527777777778" bottom="0.15625" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>